<commit_message>
reworked the check system, and worked out a few statistics on crafting check probabilities.
</commit_message>
<xml_diff>
--- a/Enchantments/Enchantments.xlsx
+++ b/Enchantments/Enchantments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charles\Documents\Git Repositories\materials_and_crafting\Enchantments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE6C267C-3FF9-4D74-8E07-A19495FE4514}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72B15695-53DA-49C1-BEA4-CBE04A4F09F2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{11AE916A-0CE2-4C8E-9116-BD67A671ABA1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="1" xr2:uid="{11AE916A-0CE2-4C8E-9116-BD67A671ABA1}"/>
   </bookViews>
   <sheets>
     <sheet name="Point Buy" sheetId="4" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="358">
   <si>
     <t>−</t>
   </si>
@@ -1220,49 +1220,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>[MIN({MCI</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>} ... {MCI</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>n</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>}) * n] MCI</t>
-    </r>
-  </si>
-  <si>
     <t>Change status condition</t>
   </si>
   <si>
@@ -1963,6 +1920,189 @@
   </si>
   <si>
     <t>[3 * CEIL({CLASS LEVEL} / 2)] MCI</t>
+  </si>
+  <si>
+    <r>
+      <t>[MIN({MCI</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>} ... {MCI</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>}) * MAX(0.5, n - 1)] MCI</t>
+    </r>
+  </si>
+  <si>
+    <t>Unique enchantment specific effect</t>
+  </si>
+  <si>
+    <t>*Not always the case.</t>
+  </si>
+  <si>
+    <t>[3 * {SPELL LEVEL}] MCI*</t>
+  </si>
+  <si>
+    <t>10TH-LEVEL MAGIC WEAPON</t>
+  </si>
+  <si>
+    <t>12TH-LEVEL MAGIC WEAPON</t>
+  </si>
+  <si>
+    <r>
+      <t>Cast the spell (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-36 MCI</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Cast the spell (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-30 MCI</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>+5 weapon</t>
+  </si>
+  <si>
+    <t>+6 weapon</t>
+  </si>
+  <si>
+    <t>58 MCI</t>
+  </si>
+  <si>
+    <r>
+      <t>Concentration (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-11 MCI</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Concentration (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-13 MCI</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2099,7 +2239,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -2209,12 +2349,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2265,26 +2414,151 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2292,145 +2566,29 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2754,10 +2912,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55E34FB7-A163-4E1A-8D89-59CF44F6A322}">
-  <dimension ref="A1:J90"/>
+  <dimension ref="A1:J91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:D11"/>
+    <sheetView topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="C91" sqref="A88:D91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2768,14 +2926,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61" t="s">
+      <c r="B1" s="41"/>
+      <c r="C1" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="61"/>
+      <c r="D1" s="41"/>
       <c r="F1" s="4" t="s">
         <v>56</v>
       </c>
@@ -2783,18 +2941,18 @@
         <v>39</v>
       </c>
       <c r="H1" s="28" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I1" s="13"/>
       <c r="J1" s="6"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="77" t="s">
+      <c r="A2" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="77"/>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
       <c r="F2" t="s">
         <v>55</v>
       </c>
@@ -2808,12 +2966,12 @@
       <c r="J2" s="6"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="60" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="59"/>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
       <c r="F3" t="s">
         <v>132</v>
       </c>
@@ -2827,14 +2985,14 @@
       <c r="J3" s="6"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="36" t="s">
         <v>97</v>
       </c>
-      <c r="B4" s="43"/>
-      <c r="C4" s="32" t="s">
+      <c r="B4" s="36"/>
+      <c r="C4" s="51" t="s">
         <v>120</v>
       </c>
-      <c r="D4" s="32"/>
+      <c r="D4" s="51"/>
       <c r="F4" t="s">
         <v>133</v>
       </c>
@@ -2848,14 +3006,14 @@
       <c r="J4" s="6"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="36" t="s">
         <v>98</v>
       </c>
-      <c r="B5" s="43"/>
-      <c r="C5" s="32" t="s">
+      <c r="B5" s="36"/>
+      <c r="C5" s="51" t="s">
         <v>95</v>
       </c>
-      <c r="D5" s="32"/>
+      <c r="D5" s="51"/>
       <c r="F5" t="s">
         <v>134</v>
       </c>
@@ -2869,178 +3027,178 @@
       <c r="J5" s="6"/>
     </row>
     <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="61" t="s">
+      <c r="A6" s="41" t="s">
         <v>115</v>
       </c>
-      <c r="B6" s="61"/>
-      <c r="C6" s="61"/>
-      <c r="D6" s="61"/>
-      <c r="F6" s="75" t="s">
+      <c r="B6" s="41"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41"/>
+      <c r="F6" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="G6" s="75">
+      <c r="G6" s="30">
         <v>56</v>
       </c>
-      <c r="H6" s="76">
+      <c r="H6" s="31">
         <v>45</v>
       </c>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="36" t="s">
         <v>116</v>
       </c>
-      <c r="B7" s="43"/>
-      <c r="C7" s="31" t="s">
-        <v>345</v>
-      </c>
-      <c r="D7" s="31"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="37" t="s">
+        <v>344</v>
+      </c>
+      <c r="D7" s="37"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
     </row>
     <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="43" t="s">
+      <c r="A8" s="36" t="s">
         <v>117</v>
       </c>
-      <c r="B8" s="43"/>
-      <c r="C8" s="31" t="s">
+      <c r="B8" s="36"/>
+      <c r="C8" s="37" t="s">
         <v>118</v>
       </c>
-      <c r="D8" s="31"/>
-      <c r="F8" s="61" t="s">
+      <c r="D8" s="37"/>
+      <c r="F8" s="41" t="s">
         <v>262</v>
       </c>
-      <c r="G8" s="61"/>
+      <c r="G8" s="41"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="43" t="s">
+      <c r="A9" s="36" t="s">
         <v>119</v>
       </c>
-      <c r="B9" s="43"/>
-      <c r="C9" s="31" t="s">
+      <c r="B9" s="36"/>
+      <c r="C9" s="37" t="s">
         <v>121</v>
       </c>
-      <c r="D9" s="31"/>
-      <c r="F9" s="64" t="s">
+      <c r="D9" s="37"/>
+      <c r="F9" s="42" t="s">
         <v>263</v>
       </c>
-      <c r="G9" s="34"/>
+      <c r="G9" s="43"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
     </row>
     <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="43" t="s">
+      <c r="A10" s="36" t="s">
         <v>294</v>
       </c>
-      <c r="B10" s="43"/>
-      <c r="C10" s="63" t="s">
-        <v>297</v>
-      </c>
-      <c r="D10" s="45"/>
-      <c r="F10" s="65" t="s">
+      <c r="B10" s="36"/>
+      <c r="C10" s="62" t="s">
+        <v>345</v>
+      </c>
+      <c r="D10" s="63"/>
+      <c r="F10" s="44" t="s">
         <v>264</v>
       </c>
-      <c r="G10" s="34"/>
+      <c r="G10" s="43"/>
     </row>
     <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="61" t="s">
+      <c r="A11" s="41" t="s">
         <v>288</v>
       </c>
-      <c r="B11" s="61"/>
-      <c r="C11" s="61"/>
-      <c r="D11" s="61"/>
-      <c r="F11" s="34" t="s">
+      <c r="B11" s="41"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="41"/>
+      <c r="F11" s="43" t="s">
         <v>266</v>
       </c>
-      <c r="G11" s="34"/>
+      <c r="G11" s="43"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="43" t="s">
+      <c r="A12" s="36" t="s">
         <v>109</v>
       </c>
-      <c r="B12" s="43"/>
-      <c r="C12" s="41" t="s">
+      <c r="B12" s="36"/>
+      <c r="C12" s="47" t="s">
         <v>284</v>
       </c>
-      <c r="D12" s="41"/>
-      <c r="F12" s="51" t="s">
+      <c r="D12" s="47"/>
+      <c r="F12" s="45" t="s">
         <v>265</v>
       </c>
-      <c r="G12" s="51"/>
+      <c r="G12" s="45"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="43" t="s">
+      <c r="A13" s="36" t="s">
         <v>110</v>
       </c>
-      <c r="B13" s="43"/>
-      <c r="C13" s="41" t="s">
+      <c r="B13" s="36"/>
+      <c r="C13" s="47" t="s">
         <v>283</v>
       </c>
-      <c r="D13" s="41"/>
-      <c r="F13" s="66" t="s">
+      <c r="D13" s="47"/>
+      <c r="F13" s="46" t="s">
         <v>275</v>
       </c>
-      <c r="G13" s="66"/>
+      <c r="G13" s="46"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="43" t="s">
+      <c r="A14" s="36" t="s">
         <v>295</v>
       </c>
-      <c r="B14" s="43"/>
-      <c r="C14" s="41" t="s">
+      <c r="B14" s="36"/>
+      <c r="C14" s="47" t="s">
         <v>96</v>
       </c>
-      <c r="D14" s="41"/>
-      <c r="F14" s="72" t="s">
+      <c r="D14" s="47"/>
+      <c r="F14" s="82" t="s">
         <v>273</v>
       </c>
-      <c r="G14" s="73"/>
+      <c r="G14" s="83"/>
     </row>
     <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="43" t="s">
+      <c r="A15" s="36" t="s">
         <v>282</v>
       </c>
-      <c r="B15" s="43"/>
-      <c r="C15" s="45" t="s">
+      <c r="B15" s="36"/>
+      <c r="C15" s="63" t="s">
         <v>296</v>
       </c>
-      <c r="D15" s="45"/>
-      <c r="F15" s="74"/>
-      <c r="G15" s="74"/>
+      <c r="D15" s="63"/>
+      <c r="F15" s="84"/>
+      <c r="G15" s="84"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="52" t="s">
+      <c r="A16" s="38" t="s">
         <v>111</v>
       </c>
-      <c r="B16" s="52"/>
-      <c r="C16" s="53" t="s">
+      <c r="B16" s="38"/>
+      <c r="C16" s="68" t="s">
         <v>96</v>
       </c>
-      <c r="D16" s="53"/>
+      <c r="D16" s="68"/>
       <c r="F16" s="27"/>
       <c r="G16" s="27"/>
     </row>
     <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="61" t="s">
+      <c r="A17" s="41" t="s">
         <v>287</v>
       </c>
-      <c r="B17" s="61"/>
-      <c r="C17" s="61"/>
-      <c r="D17" s="61"/>
+      <c r="B17" s="41"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
       <c r="F17" s="27"/>
       <c r="G17" s="27"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="30" t="s">
+      <c r="A18" s="55" t="s">
         <v>289</v>
       </c>
-      <c r="B18" s="30"/>
+      <c r="B18" s="55"/>
       <c r="C18" s="78" t="s">
         <v>8</v>
       </c>
@@ -3049,102 +3207,102 @@
       <c r="G18" s="27"/>
     </row>
     <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="35" t="s">
+      <c r="A19" s="77" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="35"/>
-      <c r="C19" s="36" t="s">
+      <c r="B19" s="77"/>
+      <c r="C19" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="D19" s="36"/>
+      <c r="D19" s="72"/>
       <c r="F19" s="27"/>
       <c r="G19" s="27"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="48" t="s">
-        <v>298</v>
-      </c>
-      <c r="B20" s="48"/>
-      <c r="C20" s="36" t="s">
+      <c r="A20" s="75" t="s">
+        <v>297</v>
+      </c>
+      <c r="B20" s="75"/>
+      <c r="C20" s="72" t="s">
         <v>291</v>
       </c>
-      <c r="D20" s="36"/>
+      <c r="D20" s="72"/>
       <c r="F20" s="26"/>
       <c r="G20" s="26"/>
     </row>
     <row r="21" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="48"/>
-      <c r="B21" s="48"/>
-      <c r="C21" s="46" t="s">
+      <c r="A21" s="75"/>
+      <c r="B21" s="75"/>
+      <c r="C21" s="73" t="s">
         <v>292</v>
       </c>
-      <c r="D21" s="46"/>
+      <c r="D21" s="73"/>
       <c r="F21" s="26"/>
       <c r="G21" s="26"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="48"/>
-      <c r="B22" s="48"/>
-      <c r="C22" s="36" t="s">
+      <c r="A22" s="75"/>
+      <c r="B22" s="75"/>
+      <c r="C22" s="72" t="s">
         <v>290</v>
       </c>
-      <c r="D22" s="36"/>
+      <c r="D22" s="72"/>
     </row>
     <row r="23" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="49"/>
-      <c r="B23" s="49"/>
-      <c r="C23" s="47" t="s">
+      <c r="A23" s="76"/>
+      <c r="B23" s="76"/>
+      <c r="C23" s="74" t="s">
         <v>293</v>
       </c>
-      <c r="D23" s="47"/>
+      <c r="D23" s="74"/>
     </row>
     <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="61" t="s">
+      <c r="A24" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="61"/>
-      <c r="C24" s="61"/>
-      <c r="D24" s="61"/>
+      <c r="B24" s="41"/>
+      <c r="C24" s="41"/>
+      <c r="D24" s="41"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="30" t="s">
+      <c r="A25" s="55" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="43"/>
-      <c r="C25" s="32" t="s">
+      <c r="B25" s="36"/>
+      <c r="C25" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="D25" s="32"/>
+      <c r="D25" s="51"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="30" t="s">
+      <c r="A26" s="55" t="s">
         <v>277</v>
       </c>
-      <c r="B26" s="30"/>
-      <c r="C26" s="31" t="s">
+      <c r="B26" s="55"/>
+      <c r="C26" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="D26" s="32"/>
+      <c r="D26" s="51"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="30" t="s">
+      <c r="A27" s="55" t="s">
         <v>281</v>
       </c>
-      <c r="B27" s="30"/>
-      <c r="C27" s="31" t="s">
+      <c r="B27" s="55"/>
+      <c r="C27" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="D27" s="32"/>
+      <c r="D27" s="51"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="62" t="s">
+      <c r="A28" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="B28" s="62"/>
-      <c r="C28" s="59" t="s">
+      <c r="B28" s="59"/>
+      <c r="C28" s="60" t="s">
         <v>73</v>
       </c>
-      <c r="D28" s="59"/>
+      <c r="D28" s="60"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
@@ -3184,7 +3342,7 @@
       <c r="C31" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D31" s="70" t="s">
+      <c r="D31" s="56" t="s">
         <v>71</v>
       </c>
     </row>
@@ -3198,100 +3356,100 @@
       <c r="C32" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D32" s="39"/>
+      <c r="D32" s="57"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="30" t="s">
+      <c r="A33" s="55" t="s">
         <v>67</v>
       </c>
-      <c r="B33" s="43"/>
-      <c r="C33" s="31" t="s">
+      <c r="B33" s="36"/>
+      <c r="C33" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="D33" s="31"/>
+      <c r="D33" s="37"/>
     </row>
     <row r="34" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="61" t="s">
+      <c r="A34" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="B34" s="61"/>
-      <c r="C34" s="61"/>
-      <c r="D34" s="61"/>
+      <c r="B34" s="41"/>
+      <c r="C34" s="41"/>
+      <c r="D34" s="41"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="79" t="s">
+      <c r="A35" s="87" t="s">
         <v>11</v>
       </c>
-      <c r="B35" s="79"/>
-      <c r="C35" s="32" t="s">
+      <c r="B35" s="87"/>
+      <c r="C35" s="86" t="s">
         <v>135</v>
       </c>
-      <c r="D35" s="31"/>
-      <c r="F35" t="s">
+      <c r="D35" s="86"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="80" t="s">
+        <v>10</v>
+      </c>
+      <c r="B36" s="80"/>
+      <c r="C36" s="81" t="s">
+        <v>136</v>
+      </c>
+      <c r="D36" s="81"/>
+    </row>
+    <row r="37" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="B37" s="41"/>
+      <c r="C37" s="41"/>
+      <c r="D37" s="41"/>
+      <c r="F37" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="37" t="s">
-        <v>10</v>
-      </c>
-      <c r="B36" s="37"/>
-      <c r="C36" s="38" t="s">
-        <v>136</v>
-      </c>
-      <c r="D36" s="38"/>
-    </row>
-    <row r="37" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="61" t="s">
-        <v>21</v>
-      </c>
-      <c r="B37" s="61"/>
-      <c r="C37" s="61"/>
-      <c r="D37" s="61"/>
-    </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="43" t="s">
+      <c r="A38" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="B38" s="43"/>
-      <c r="C38" s="44" t="s">
+      <c r="B38" s="36"/>
+      <c r="C38" s="61" t="s">
         <v>26</v>
       </c>
-      <c r="D38" s="44"/>
+      <c r="D38" s="61"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="60" t="s">
+      <c r="A39" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="B39" s="60"/>
-      <c r="C39" s="44" t="s">
+      <c r="B39" s="49"/>
+      <c r="C39" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="D39" s="44"/>
+      <c r="D39" s="61"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="60" t="s">
+      <c r="A40" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="B40" s="60"/>
-      <c r="C40" s="44" t="s">
+      <c r="B40" s="49"/>
+      <c r="C40" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="D40" s="44"/>
+      <c r="D40" s="61"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="39" t="s">
+      <c r="A41" s="57" t="s">
         <v>99</v>
       </c>
-      <c r="B41" s="39"/>
-      <c r="C41" s="34" t="s">
+      <c r="B41" s="57"/>
+      <c r="C41" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="D41" s="34"/>
+      <c r="D41" s="43"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="39"/>
-      <c r="B42" s="39"/>
+      <c r="A42" s="57"/>
+      <c r="B42" s="57"/>
       <c r="C42" s="9" t="s">
         <v>43</v>
       </c>
@@ -3300,40 +3458,40 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="39"/>
-      <c r="B43" s="39"/>
+      <c r="A43" s="57"/>
+      <c r="B43" s="57"/>
       <c r="C43" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D43" s="57" t="s">
+      <c r="D43" s="65" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="71"/>
-      <c r="B44" s="71"/>
+      <c r="A44" s="58"/>
+      <c r="B44" s="58"/>
       <c r="C44" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="D44" s="58"/>
+      <c r="D44" s="66"/>
     </row>
     <row r="45" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="61" t="s">
+      <c r="A45" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="B45" s="61"/>
-      <c r="C45" s="61"/>
-      <c r="D45" s="61"/>
+      <c r="B45" s="41"/>
+      <c r="C45" s="41"/>
+      <c r="D45" s="41"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="43" t="s">
+      <c r="A46" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="B46" s="43"/>
-      <c r="C46" s="31" t="s">
+      <c r="B46" s="36"/>
+      <c r="C46" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="D46" s="69"/>
+      <c r="D46" s="54"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
@@ -3350,312 +3508,312 @@
       </c>
     </row>
     <row r="48" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="61" t="s">
+      <c r="A48" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="B48" s="61"/>
-      <c r="C48" s="61"/>
-      <c r="D48" s="61"/>
+      <c r="B48" s="41"/>
+      <c r="C48" s="41"/>
+      <c r="D48" s="41"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="43" t="s">
+      <c r="A49" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="B49" s="43"/>
-      <c r="C49" s="41" t="s">
+      <c r="B49" s="36"/>
+      <c r="C49" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="D49" s="42"/>
+      <c r="D49" s="52"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="43" t="s">
+      <c r="A50" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="B50" s="43"/>
-      <c r="C50" s="59" t="s">
+      <c r="B50" s="36"/>
+      <c r="C50" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="D50" s="59"/>
+      <c r="D50" s="60"/>
     </row>
     <row r="51" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="61" t="s">
+      <c r="A51" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="B51" s="61"/>
-      <c r="C51" s="61"/>
-      <c r="D51" s="61"/>
+      <c r="B51" s="41"/>
+      <c r="C51" s="41"/>
+      <c r="D51" s="41"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="43" t="s">
+      <c r="A52" s="36" t="s">
         <v>270</v>
       </c>
-      <c r="B52" s="43"/>
-      <c r="C52" s="32" t="s">
+      <c r="B52" s="36"/>
+      <c r="C52" s="51" t="s">
         <v>96</v>
       </c>
-      <c r="D52" s="32"/>
+      <c r="D52" s="51"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="43" t="s">
+      <c r="A53" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="B53" s="43"/>
-      <c r="C53" s="39" t="s">
+      <c r="B53" s="36"/>
+      <c r="C53" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="D53" s="39"/>
+      <c r="D53" s="57"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="43" t="s">
+      <c r="A54" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="B54" s="43"/>
-      <c r="C54" s="39"/>
-      <c r="D54" s="39"/>
+      <c r="B54" s="36"/>
+      <c r="C54" s="57"/>
+      <c r="D54" s="57"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="33" t="s">
+      <c r="A55" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="B55" s="33"/>
-      <c r="C55" s="34" t="s">
+      <c r="B55" s="53"/>
+      <c r="C55" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="D55" s="34"/>
+      <c r="D55" s="43"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="33" t="s">
+      <c r="A56" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="B56" s="33"/>
-      <c r="C56" s="34" t="s">
+      <c r="B56" s="53"/>
+      <c r="C56" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="D56" s="34"/>
+      <c r="D56" s="43"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="33" t="s">
+      <c r="A57" s="53" t="s">
         <v>280</v>
       </c>
-      <c r="B57" s="33"/>
-      <c r="C57" s="34" t="s">
+      <c r="B57" s="53"/>
+      <c r="C57" s="43" t="s">
         <v>279</v>
       </c>
-      <c r="D57" s="34"/>
+      <c r="D57" s="43"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="33" t="s">
+      <c r="A58" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="B58" s="33"/>
-      <c r="C58" s="34" t="s">
+      <c r="B58" s="53"/>
+      <c r="C58" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="D58" s="34"/>
+      <c r="D58" s="43"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="33" t="s">
+      <c r="A59" s="53" t="s">
         <v>278</v>
       </c>
-      <c r="B59" s="33"/>
-      <c r="C59" s="34" t="s">
+      <c r="B59" s="53"/>
+      <c r="C59" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="D59" s="34"/>
+      <c r="D59" s="43"/>
     </row>
     <row r="60" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="61" t="s">
+      <c r="A60" s="41" t="s">
         <v>103</v>
       </c>
-      <c r="B60" s="61"/>
-      <c r="C60" s="61"/>
-      <c r="D60" s="61"/>
+      <c r="B60" s="41"/>
+      <c r="C60" s="41"/>
+      <c r="D60" s="41"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="30" t="s">
+      <c r="A61" s="55" t="s">
         <v>104</v>
       </c>
-      <c r="B61" s="30"/>
-      <c r="C61" s="80" t="s">
+      <c r="B61" s="55"/>
+      <c r="C61" s="79" t="s">
         <v>271</v>
       </c>
-      <c r="D61" s="44"/>
+      <c r="D61" s="61"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="43" t="s">
+      <c r="A62" s="36" t="s">
         <v>268</v>
       </c>
-      <c r="B62" s="43"/>
-      <c r="C62" s="32" t="s">
+      <c r="B62" s="36"/>
+      <c r="C62" s="51" t="s">
         <v>269</v>
       </c>
-      <c r="D62" s="32"/>
+      <c r="D62" s="51"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="43" t="s">
+      <c r="A63" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="B63" s="43"/>
-      <c r="C63" s="44" t="s">
+      <c r="B63" s="36"/>
+      <c r="C63" s="61" t="s">
         <v>106</v>
       </c>
-      <c r="D63" s="44"/>
+      <c r="D63" s="61"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="43" t="s">
+      <c r="A64" s="36" t="s">
         <v>286</v>
       </c>
-      <c r="B64" s="43"/>
-      <c r="C64" s="32" t="s">
+      <c r="B64" s="36"/>
+      <c r="C64" s="51" t="s">
         <v>269</v>
       </c>
-      <c r="D64" s="32"/>
+      <c r="D64" s="51"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="43" t="s">
+      <c r="A65" s="36" t="s">
         <v>267</v>
       </c>
-      <c r="B65" s="43"/>
-      <c r="C65" s="41" t="s">
+      <c r="B65" s="36"/>
+      <c r="C65" s="47" t="s">
         <v>96</v>
       </c>
-      <c r="D65" s="42"/>
+      <c r="D65" s="52"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="43" t="s">
+      <c r="A66" s="36" t="s">
         <v>285</v>
       </c>
-      <c r="B66" s="43"/>
-      <c r="C66" s="41" t="s">
+      <c r="B66" s="36"/>
+      <c r="C66" s="47" t="s">
         <v>96</v>
       </c>
-      <c r="D66" s="42"/>
+      <c r="D66" s="52"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="43" t="s">
+      <c r="A67" s="36" t="s">
         <v>107</v>
       </c>
-      <c r="B67" s="43"/>
-      <c r="C67" s="41" t="s">
+      <c r="B67" s="36"/>
+      <c r="C67" s="47" t="s">
         <v>95</v>
       </c>
-      <c r="D67" s="42"/>
+      <c r="D67" s="52"/>
     </row>
     <row r="68" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="61" t="s">
+      <c r="A68" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="B68" s="61"/>
-      <c r="C68" s="61"/>
-      <c r="D68" s="61"/>
+      <c r="B68" s="41"/>
+      <c r="C68" s="41"/>
+      <c r="D68" s="41"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="33" t="s">
+      <c r="A69" s="53" t="s">
         <v>79</v>
       </c>
-      <c r="B69" s="33"/>
-      <c r="C69" s="39" t="s">
+      <c r="B69" s="53"/>
+      <c r="C69" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="D69" s="39"/>
+      <c r="D69" s="57"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="33" t="s">
+      <c r="A70" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="B70" s="33"/>
-      <c r="C70" s="39"/>
-      <c r="D70" s="39"/>
+      <c r="B70" s="53"/>
+      <c r="C70" s="57"/>
+      <c r="D70" s="57"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="33" t="s">
+      <c r="A71" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="B71" s="33"/>
-      <c r="C71" s="39" t="s">
+      <c r="B71" s="53"/>
+      <c r="C71" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="D71" s="39"/>
+      <c r="D71" s="57"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="33" t="s">
+      <c r="A72" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="B72" s="33"/>
-      <c r="C72" s="39"/>
-      <c r="D72" s="39"/>
+      <c r="B72" s="53"/>
+      <c r="C72" s="57"/>
+      <c r="D72" s="57"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="33" t="s">
+      <c r="A73" s="53" t="s">
         <v>83</v>
       </c>
-      <c r="B73" s="33"/>
-      <c r="C73" s="54" t="s">
+      <c r="B73" s="53"/>
+      <c r="C73" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="D73" s="54"/>
+      <c r="D73" s="69"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="33" t="s">
+      <c r="A74" s="53" t="s">
         <v>84</v>
       </c>
-      <c r="B74" s="33"/>
-      <c r="C74" s="54"/>
-      <c r="D74" s="54"/>
+      <c r="B74" s="53"/>
+      <c r="C74" s="69"/>
+      <c r="D74" s="69"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="33" t="s">
+      <c r="A75" s="53" t="s">
         <v>85</v>
       </c>
-      <c r="B75" s="33"/>
-      <c r="C75" s="34" t="s">
+      <c r="B75" s="53"/>
+      <c r="C75" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="D75" s="34"/>
+      <c r="D75" s="43"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="33" t="s">
+      <c r="A76" s="53" t="s">
         <v>86</v>
       </c>
-      <c r="B76" s="33"/>
-      <c r="C76" s="34" t="s">
+      <c r="B76" s="53"/>
+      <c r="C76" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="D76" s="34"/>
+      <c r="D76" s="43"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="33" t="s">
+      <c r="A77" s="53" t="s">
         <v>87</v>
       </c>
-      <c r="B77" s="33"/>
-      <c r="C77" s="34" t="s">
+      <c r="B77" s="53"/>
+      <c r="C77" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="D77" s="34"/>
+      <c r="D77" s="43"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="33" t="s">
+      <c r="A78" s="53" t="s">
         <v>88</v>
       </c>
-      <c r="B78" s="33"/>
-      <c r="C78" s="34" t="s">
+      <c r="B78" s="53"/>
+      <c r="C78" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="D78" s="34"/>
+      <c r="D78" s="43"/>
     </row>
     <row r="79" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="61" t="s">
+      <c r="A79" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="B79" s="61"/>
-      <c r="C79" s="61"/>
-      <c r="D79" s="61"/>
+      <c r="B79" s="41"/>
+      <c r="C79" s="41"/>
+      <c r="D79" s="41"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="39" t="s">
+      <c r="A80" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="B80" s="39"/>
+      <c r="B80" s="57"/>
       <c r="C80" s="11" t="s">
         <v>122</v>
       </c>
@@ -3663,9 +3821,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="39"/>
-      <c r="B81" s="39"/>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="57"/>
+      <c r="B81" s="57"/>
       <c r="C81" s="21" t="s">
         <v>123</v>
       </c>
@@ -3673,118 +3831,208 @@
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="60" t="s">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="B82" s="60"/>
-      <c r="C82" s="41" t="s">
+      <c r="B82" s="49"/>
+      <c r="C82" s="47" t="s">
+        <v>299</v>
+      </c>
+      <c r="D82" s="48"/>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" s="49" t="s">
+        <v>124</v>
+      </c>
+      <c r="B83" s="49"/>
+      <c r="C83" s="47" t="s">
         <v>300</v>
       </c>
-      <c r="D82" s="67"/>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="60" t="s">
-        <v>124</v>
-      </c>
-      <c r="B83" s="60"/>
-      <c r="C83" s="41" t="s">
-        <v>301</v>
-      </c>
-      <c r="D83" s="67"/>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="68" t="s">
+      <c r="D83" s="48"/>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" s="50" t="s">
         <v>272</v>
       </c>
-      <c r="B84" s="68"/>
-      <c r="C84" s="31" t="s">
+      <c r="B84" s="50"/>
+      <c r="C84" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="D84" s="69"/>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="68"/>
-      <c r="B85" s="68"/>
-      <c r="C85" s="32" t="s">
+      <c r="D84" s="54"/>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" s="50"/>
+      <c r="B85" s="50"/>
+      <c r="C85" s="51" t="s">
         <v>126</v>
       </c>
-      <c r="D85" s="42"/>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="52" t="s">
+      <c r="D85" s="52"/>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="B86" s="52"/>
-      <c r="C86" s="55" t="s">
+      <c r="B86" s="38"/>
+      <c r="C86" s="70" t="s">
         <v>108</v>
       </c>
-      <c r="D86" s="56"/>
-    </row>
-    <row r="87" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="61" t="s">
+      <c r="D86" s="71"/>
+    </row>
+    <row r="87" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="41" t="s">
         <v>94</v>
       </c>
-      <c r="B87" s="61"/>
-      <c r="C87" s="61"/>
-      <c r="D87" s="61"/>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="33" t="s">
+      <c r="B87" s="41"/>
+      <c r="C87" s="41"/>
+      <c r="D87" s="41"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" s="89" t="s">
+        <v>346</v>
+      </c>
+      <c r="B88" s="89"/>
+      <c r="C88" s="88" t="s">
+        <v>348</v>
+      </c>
+      <c r="D88" s="88"/>
+      <c r="F88" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" s="53" t="s">
         <v>92</v>
       </c>
-      <c r="B88" s="33"/>
-      <c r="C88" s="50" t="s">
+      <c r="B89" s="53"/>
+      <c r="C89" s="67" t="s">
         <v>93</v>
       </c>
-      <c r="D88" s="51"/>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="33" t="s">
+      <c r="D89" s="45"/>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" s="53" t="s">
         <v>113</v>
       </c>
-      <c r="B89" s="33"/>
-      <c r="C89" s="41" t="s">
+      <c r="B90" s="53"/>
+      <c r="C90" s="47" t="s">
         <v>114</v>
       </c>
-      <c r="D89" s="41"/>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="52" t="s">
+      <c r="D90" s="47"/>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" s="38" t="s">
         <v>137</v>
       </c>
-      <c r="B90" s="52"/>
-      <c r="C90" s="81" t="s">
+      <c r="B91" s="38"/>
+      <c r="C91" s="39" t="s">
         <v>276</v>
       </c>
-      <c r="D90" s="82"/>
+      <c r="D91" s="40"/>
     </row>
   </sheetData>
-  <mergeCells count="147">
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="C90:D90"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="C82:D82"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="A84:B85"/>
-    <mergeCell ref="C85:D85"/>
+  <mergeCells count="149">
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="C88:D88"/>
+    <mergeCell ref="F14:G15"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="A80:B81"/>
+    <mergeCell ref="A60:D60"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="A20:B23"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="A79:D79"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
     <mergeCell ref="A89:B89"/>
     <mergeCell ref="C89:D89"/>
-    <mergeCell ref="C84:D84"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="A24:D24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="A37:D37"/>
-    <mergeCell ref="A41:B44"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="C76:D76"/>
+    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="C73:D74"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="A87:D87"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="A68:D68"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="C71:D72"/>
+    <mergeCell ref="C69:D70"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="C53:D54"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A48:D48"/>
+    <mergeCell ref="A45:D45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="A51:D51"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="A62:B62"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="A17:D17"/>
@@ -3809,105 +4057,30 @@
     <mergeCell ref="A6:D6"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C71:D72"/>
-    <mergeCell ref="C69:D70"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="C53:D54"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A48:D48"/>
-    <mergeCell ref="A45:D45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="A51:D51"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="C88:D88"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="C77:D77"/>
-    <mergeCell ref="C76:D76"/>
-    <mergeCell ref="C75:D75"/>
-    <mergeCell ref="C73:D74"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="A87:D87"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="A68:D68"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="A80:B81"/>
-    <mergeCell ref="A60:D60"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="A20:B23"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="A79:D79"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="F14:G15"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="C91:D91"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="C82:D82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="C83:D83"/>
+    <mergeCell ref="A84:B85"/>
+    <mergeCell ref="C85:D85"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="C90:D90"/>
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="A41:B44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3916,10 +4089,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADDC067E-E059-49F6-9F6D-C61CC1C32937}">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:B22"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3929,10 +4102,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="85" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="40"/>
+      <c r="B1" s="85"/>
       <c r="C1" s="10"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -3982,10 +4155,10 @@
       <c r="C7" s="10"/>
     </row>
     <row r="8" spans="1:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="40" t="s">
+      <c r="A8" s="85" t="s">
         <v>61</v>
       </c>
-      <c r="B8" s="40"/>
+      <c r="B8" s="85"/>
       <c r="C8" s="16"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -4029,10 +4202,10 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="40" t="s">
+      <c r="A15" s="85" t="s">
         <v>65</v>
       </c>
-      <c r="B15" s="40"/>
+      <c r="B15" s="85"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
@@ -4075,22 +4248,22 @@
       </c>
     </row>
     <row r="22" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="40" t="s">
-        <v>336</v>
-      </c>
-      <c r="B22" s="40"/>
+      <c r="A22" s="85" t="s">
+        <v>335</v>
+      </c>
+      <c r="B22" s="85"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B24" s="19" t="s">
         <v>1</v>
@@ -4114,18 +4287,112 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="20" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B27" s="20" t="s">
         <v>59</v>
       </c>
     </row>
+    <row r="29" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="85" t="s">
+        <v>349</v>
+      </c>
+      <c r="B29" s="85"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="14" t="s">
+        <v>352</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B32" s="18" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B33" s="18" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="20" t="s">
+        <v>330</v>
+      </c>
+      <c r="B34" s="20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="85" t="s">
+        <v>350</v>
+      </c>
+      <c r="B36" s="85"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="14" t="s">
+        <v>351</v>
+      </c>
+      <c r="B37" s="15" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="B38" s="19" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B39" s="18" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B40" s="18" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="20" t="s">
+        <v>355</v>
+      </c>
+      <c r="B41" s="20" t="s">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
+    <mergeCell ref="A36:B36"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A29:B29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4135,331 +4402,331 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38047AC7-8B1B-4A43-A073-1FEFCCB73D34}">
   <dimension ref="A1:B52"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.28515625" customWidth="1"/>
-    <col min="2" max="2" width="34.28515625" style="86" customWidth="1"/>
+    <col min="2" max="2" width="34.28515625" style="35" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="61" t="s">
-        <v>311</v>
-      </c>
-      <c r="B1" s="61"/>
+      <c r="A1" s="41" t="s">
+        <v>310</v>
+      </c>
+      <c r="B1" s="41"/>
     </row>
     <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
-        <v>309</v>
-      </c>
-      <c r="B2" s="83" t="s">
-        <v>306</v>
+        <v>308</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>304</v>
-      </c>
-      <c r="B3" s="84" t="s">
         <v>303</v>
+      </c>
+      <c r="B3" s="33" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
-        <v>310</v>
-      </c>
-      <c r="B4" s="85" t="s">
+        <v>309</v>
+      </c>
+      <c r="B4" s="34" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="61" t="s">
-        <v>312</v>
-      </c>
-      <c r="B6" s="61"/>
+      <c r="A6" s="41" t="s">
+        <v>311</v>
+      </c>
+      <c r="B6" s="41"/>
     </row>
     <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
-        <v>313</v>
-      </c>
-      <c r="B7" s="83" t="s">
-        <v>306</v>
+        <v>312</v>
+      </c>
+      <c r="B7" s="32" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="29" t="s">
-        <v>315</v>
-      </c>
-      <c r="B8" s="84"/>
+        <v>314</v>
+      </c>
+      <c r="B8" s="33"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>304</v>
-      </c>
-      <c r="B9" s="84" t="s">
         <v>303</v>
+      </c>
+      <c r="B9" s="33" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
-        <v>314</v>
-      </c>
-      <c r="B10" s="85" t="s">
+        <v>313</v>
+      </c>
+      <c r="B10" s="34" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="61" t="s">
-        <v>319</v>
-      </c>
-      <c r="B12" s="61"/>
+      <c r="A12" s="41" t="s">
+        <v>318</v>
+      </c>
+      <c r="B12" s="41"/>
     </row>
     <row r="13" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
-        <v>316</v>
-      </c>
-      <c r="B13" s="83" t="s">
-        <v>306</v>
+        <v>315</v>
+      </c>
+      <c r="B13" s="32" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="29" t="s">
-        <v>320</v>
-      </c>
-      <c r="B14" s="84"/>
+        <v>319</v>
+      </c>
+      <c r="B14" s="33"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>304</v>
-      </c>
-      <c r="B15" s="84" t="s">
         <v>303</v>
+      </c>
+      <c r="B15" s="33" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
-        <v>317</v>
-      </c>
-      <c r="B16" s="85" t="s">
+        <v>316</v>
+      </c>
+      <c r="B16" s="34" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="61" t="s">
-        <v>322</v>
-      </c>
-      <c r="B18" s="61"/>
+      <c r="A18" s="41" t="s">
+        <v>321</v>
+      </c>
+      <c r="B18" s="41"/>
     </row>
     <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="29" t="s">
-        <v>318</v>
-      </c>
-      <c r="B19" s="83" t="s">
-        <v>306</v>
+        <v>317</v>
+      </c>
+      <c r="B19" s="32" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="29" t="s">
-        <v>321</v>
-      </c>
-      <c r="B20" s="84"/>
+        <v>320</v>
+      </c>
+      <c r="B20" s="33"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>304</v>
-      </c>
-      <c r="B21" s="84" t="s">
         <v>303</v>
+      </c>
+      <c r="B21" s="33" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="B22" s="85" t="s">
+      <c r="B22" s="34" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="61" t="s">
-        <v>308</v>
-      </c>
-      <c r="B24" s="61"/>
+      <c r="A24" s="41" t="s">
+        <v>307</v>
+      </c>
+      <c r="B24" s="41"/>
     </row>
     <row r="25" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="29" t="s">
-        <v>307</v>
-      </c>
-      <c r="B25" s="83" t="s">
         <v>306</v>
+      </c>
+      <c r="B25" s="32" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="29" t="s">
-        <v>305</v>
-      </c>
-      <c r="B26" s="84"/>
+        <v>304</v>
+      </c>
+      <c r="B26" s="33"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>304</v>
-      </c>
-      <c r="B27" s="84" t="s">
         <v>303</v>
+      </c>
+      <c r="B27" s="33" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="20" t="s">
-        <v>302</v>
-      </c>
-      <c r="B28" s="85" t="s">
+        <v>301</v>
+      </c>
+      <c r="B28" s="34" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="61" t="s">
-        <v>323</v>
-      </c>
-      <c r="B30" s="61"/>
+      <c r="A30" s="41" t="s">
+        <v>322</v>
+      </c>
+      <c r="B30" s="41"/>
     </row>
     <row r="31" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="29" t="s">
-        <v>325</v>
-      </c>
-      <c r="B31" s="83" t="s">
-        <v>306</v>
+        <v>324</v>
+      </c>
+      <c r="B31" s="32" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="29" t="s">
-        <v>341</v>
-      </c>
-      <c r="B32" s="84"/>
+        <v>340</v>
+      </c>
+      <c r="B32" s="33"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>304</v>
-      </c>
-      <c r="B33" s="84" t="s">
         <v>303</v>
+      </c>
+      <c r="B33" s="33" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="20" t="s">
-        <v>326</v>
-      </c>
-      <c r="B34" s="85" t="s">
+        <v>325</v>
+      </c>
+      <c r="B34" s="34" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="61" t="s">
-        <v>324</v>
-      </c>
-      <c r="B36" s="61"/>
+      <c r="A36" s="41" t="s">
+        <v>323</v>
+      </c>
+      <c r="B36" s="41"/>
     </row>
     <row r="37" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="29" t="s">
-        <v>328</v>
-      </c>
-      <c r="B37" s="83" t="s">
-        <v>306</v>
+        <v>327</v>
+      </c>
+      <c r="B37" s="32" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="29" t="s">
-        <v>342</v>
-      </c>
-      <c r="B38" s="84"/>
+        <v>341</v>
+      </c>
+      <c r="B38" s="33"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>304</v>
-      </c>
-      <c r="B39" s="84" t="s">
         <v>303</v>
+      </c>
+      <c r="B39" s="33" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="20" t="s">
-        <v>327</v>
-      </c>
-      <c r="B40" s="85" t="s">
+        <v>326</v>
+      </c>
+      <c r="B40" s="34" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="61" t="s">
-        <v>329</v>
-      </c>
-      <c r="B42" s="61"/>
+      <c r="A42" s="41" t="s">
+        <v>328</v>
+      </c>
+      <c r="B42" s="41"/>
     </row>
     <row r="43" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="29" t="s">
-        <v>330</v>
-      </c>
-      <c r="B43" s="83" t="s">
-        <v>306</v>
+        <v>329</v>
+      </c>
+      <c r="B43" s="32" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="29" t="s">
-        <v>343</v>
-      </c>
-      <c r="B44" s="84"/>
+        <v>342</v>
+      </c>
+      <c r="B44" s="33"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
-        <v>304</v>
-      </c>
-      <c r="B45" s="84" t="s">
         <v>303</v>
+      </c>
+      <c r="B45" s="33" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="20" t="s">
+        <v>330</v>
+      </c>
+      <c r="B46" s="34" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="41" t="s">
         <v>331</v>
       </c>
-      <c r="B46" s="85" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="61" t="s">
-        <v>332</v>
-      </c>
-      <c r="B48" s="61"/>
+      <c r="B48" s="41"/>
     </row>
     <row r="49" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="29" t="s">
-        <v>333</v>
-      </c>
-      <c r="B49" s="83" t="s">
-        <v>306</v>
+        <v>332</v>
+      </c>
+      <c r="B49" s="32" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="29" t="s">
-        <v>334</v>
-      </c>
-      <c r="B50" s="84"/>
+        <v>333</v>
+      </c>
+      <c r="B50" s="33"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
-        <v>304</v>
-      </c>
-      <c r="B51" s="84" t="s">
         <v>303</v>
+      </c>
+      <c r="B51" s="33" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="20" t="s">
-        <v>335</v>
-      </c>
-      <c r="B52" s="85" t="s">
+        <v>334</v>
+      </c>
+      <c r="B52" s="34" t="s">
         <v>60</v>
       </c>
     </row>
@@ -5327,7 +5594,7 @@
     </row>
     <row r="105" spans="1:2" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="22" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B105" s="24">
         <v>28000</v>

</xml_diff>